<commit_message>
CORREÇÕE E INICIO ORDEM DE SERVIÇO
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/RECEITA_CENTRAL_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/RECEITA_CENTRAL_MODELO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C82FE8D-1B1B-45AB-BF50-DAADE710E86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78701ED7-0DA6-44CF-973A-C6977DA9EC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,6 +379,9 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -429,9 +432,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,7 +774,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -790,70 +790,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="7"/>
       <c r="F3" s="6"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="G4" s="12" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="G4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="15"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -861,15 +861,15 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+    <row r="7" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -878,12 +878,12 @@
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="28" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="1" t="s">

</xml_diff>

<commit_message>
AJUSTES E INICIO A SISTEMA DE APONTAMENTO
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/RECEITA_CENTRAL_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/RECEITA_CENTRAL_MODELO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78701ED7-0DA6-44CF-973A-C6977DA9EC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF98DB45-9321-44A2-AF1A-89A93521D843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelo" sheetId="2" r:id="rId1"/>
@@ -135,7 +135,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -200,6 +203,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -342,8 +351,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -382,6 +392,36 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -391,51 +431,22 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="43" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -451,9 +462,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -491,9 +502,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -526,26 +537,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -578,26 +572,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -774,7 +751,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -790,70 +767,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="7"/>
       <c r="F3" s="6"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="19"/>
       <c r="D5" s="20"/>
       <c r="E5" s="21"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="16"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -862,14 +839,14 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -878,11 +855,11 @@
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="11" t="s">
         <v>9</v>
       </c>
@@ -895,6 +872,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A2:B2"/>
@@ -904,11 +886,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="98" orientation="landscape" r:id="rId1"/>

</xml_diff>